<commit_message>
Meeting Minutes Google Sheet Uploaded
</commit_message>
<xml_diff>
--- a/Meeting Minutes/Meeting Minutes.xlsx
+++ b/Meeting Minutes/Meeting Minutes.xlsx
@@ -56,7 +56,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -65,6 +65,23 @@
     </font>
     <font>
       <b/>
+      <sz val="15.0"/>
+      <color theme="1"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="15.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -89,29 +106,98 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF5B95F9"/>
+          <bgColor rgb="FF5B95F9"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE8F0FE"/>
+          <bgColor rgb="FFE8F0FE"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1">
+    <tableStyle count="3" pivot="0" name="Sheet1-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:G10" displayName="Table_1" name="Table_1" id="1">
+  <tableColumns count="7">
+    <tableColumn name="Meeting Date" id="1"/>
+    <tableColumn name="Attendees" id="2"/>
+    <tableColumn name="Agenda" id="3"/>
+    <tableColumn name="Key Discussion Points" id="4"/>
+    <tableColumn name="Decisions Made" id="5"/>
+    <tableColumn name="Action Items" id="6"/>
+    <tableColumn name="Next Meeting Date" id="7"/>
+  </tableColumns>
+  <tableStyleInfo name="Sheet1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -318,14 +404,16 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="20.63"/>
-    <col customWidth="1" min="4" max="4" width="52.38"/>
-    <col customWidth="1" min="5" max="5" width="55.88"/>
-    <col customWidth="1" min="6" max="6" width="47.63"/>
-    <col customWidth="1" min="7" max="7" width="17.0"/>
+    <col customWidth="1" min="1" max="1" width="21.25"/>
+    <col customWidth="1" min="2" max="2" width="25.75"/>
+    <col customWidth="1" min="3" max="3" width="16.25"/>
+    <col customWidth="1" min="4" max="4" width="71.25"/>
+    <col customWidth="1" min="5" max="5" width="76.13"/>
+    <col customWidth="1" min="6" max="6" width="67.0"/>
+    <col customWidth="1" min="7" max="7" width="26.75"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="30.0" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -347,52 +435,149 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>45968.0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <v>45975.0</v>
       </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="2"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8">
-      <c r="D8" s="3"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" sqref="A2:A10 G2:G10">
+      <formula1>OR(NOT(ISERROR(DATEVALUE(A2))), AND(ISNUMBER(A2), LEFT(CELL("format", A2))="D"))</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>